<commit_message>
feat(database): add platoon and week_label columns to form_responses table; create import_schemas table
feat(analytics): implement FormAnalytics service for summarizing platoon data and insights

feat(exporter): create ExcelExporter for generating platoon and battalion reports

fix(queries): update gap and ok token handling in QueryService

fix(sync): enhance sync service to track etags and schema snapshots

test: update tests to reflect changes in file names and add new analytics tests
</commit_message>
<xml_diff>
--- a/data/input/sync_tmp/platoon_loadout.xlsx
+++ b/data/input/sync_tmp/platoon_loadout.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="177">
   <si>
     <t xml:space="preserve">דוח זיווד </t>
   </si>
@@ -533,10 +533,16 @@
     <t>מרגמה 60 תאורה</t>
   </si>
   <si>
+    <t xml:space="preserve"> 1 חוסר</t>
+  </si>
+  <si>
     <t>מעיל רוח</t>
   </si>
   <si>
     <t>דוח אמצעים</t>
+  </si>
+  <si>
+    <t xml:space="preserve">חוסר חלקי </t>
   </si>
 </sst>
 </file>
@@ -3363,7 +3369,7 @@
         <v>1.0</v>
       </c>
       <c r="H26" s="15">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="I26" s="15">
         <v>1.0</v>
@@ -4486,7 +4492,7 @@
         <v>1.0</v>
       </c>
       <c r="H42" s="15">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="I42" s="15">
         <v>1.0</v>
@@ -8766,7 +8772,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <pane ySplit="2.0" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B4" sqref="B4" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
@@ -9508,8 +9517,8 @@
       <c r="G13" s="70" t="s">
         <v>166</v>
       </c>
-      <c r="H13" s="70" t="s">
-        <v>166</v>
+      <c r="H13" s="71" t="s">
+        <v>173</v>
       </c>
       <c r="I13" s="70" t="s">
         <v>166</v>
@@ -9528,7 +9537,7 @@
       </c>
       <c r="N13" s="70"/>
       <c r="P13" s="31" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="Q13" s="32">
         <v>6.0</v>
@@ -9792,7 +9801,7 @@
       </c>
       <c r="N18" s="70"/>
       <c r="P18" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="Q18" s="5"/>
       <c r="R18" s="5"/>
@@ -9830,8 +9839,8 @@
       <c r="G19" s="70" t="s">
         <v>166</v>
       </c>
-      <c r="H19" s="70" t="s">
-        <v>166</v>
+      <c r="H19" s="71" t="s">
+        <v>176</v>
       </c>
       <c r="I19" s="70" t="s">
         <v>166</v>
@@ -14742,8 +14751,11 @@
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C13:M13">
       <formula1>"קיים,1 בלאי,2 בלאי, 1 חוסר,2 חוסר"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C3:M12 C14:M68">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C3:M12 C14:M18 C19:G19 I19:M19 C20:M68">
       <formula1>"קיים,בלאי,חוסר"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H19">
+      <formula1>"קיים,בלאי,חוסר,חוסר חלקי "</formula1>
     </dataValidation>
   </dataValidations>
   <drawing r:id="rId1"/>

</xml_diff>